<commit_message>
ensuring compatibility with the accidentally modified TMH
</commit_message>
<xml_diff>
--- a/data-raw/R2R_TMH_habitat_inputs/Cleaned Floodplain Width Calculations.xlsx
+++ b/data-raw/R2R_TMH_habitat_inputs/Cleaned Floodplain Width Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/R2R/DSMhabitat/data-raw/R2R_TMH_habitat_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED86C61A-FA5F-5744-A3F6-6422756CCCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA76559-8422-2948-958F-EED0F224D52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Above Dam" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Camanche Reservoir
@@ -60,7 +59,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>pardee dam
@@ -75,7 +73,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>clear creek dam
@@ -90,7 +87,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>north fork
@@ -105,7 +101,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>south fork
@@ -120,7 +115,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>south fork
@@ -135,7 +129,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>middle fork
@@ -150,7 +143,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>north fork
@@ -331,7 +323,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -342,46 +334,27 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -430,8 +403,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,9 +623,9 @@
   </sheetPr>
   <dimension ref="A1:I263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I169" sqref="I169"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2917,13 +2888,12 @@
       <c r="D163" s="2">
         <v>26305.41</v>
       </c>
-      <c r="E163" s="14">
-        <f>(180+37.23) * 5280</f>
-        <v>1146974.3999999999</v>
+      <c r="E163" s="6">
+        <v>241190.39999999999</v>
       </c>
       <c r="F163" s="3">
-        <f>(E163-G163-H163)/5280</f>
-        <v>208.7822727272727</v>
+        <f t="shared" si="1"/>
+        <v>37.232272727272729</v>
       </c>
       <c r="G163" s="1">
         <v>44604</v>
@@ -2993,7 +2963,6 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H167" s="14"/>
     </row>
     <row r="168" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
@@ -4247,8 +4216,8 @@
   </sheetPr>
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H106" sqref="H106"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4279,7 +4248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -4300,7 +4269,7 @@
         <v>58.39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -4314,7 +4283,7 @@
         <v>17148.54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -4328,7 +4297,7 @@
         <v>17899.47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -4336,7 +4305,7 @@
         <v>54.56</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -4344,7 +4313,7 @@
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -4352,7 +4321,7 @@
         <v>70.55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -4360,7 +4329,7 @@
         <v>116.37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -4368,7 +4337,7 @@
         <v>98.01</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +4345,7 @@
         <v>84.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -4384,7 +4353,7 @@
         <v>113.12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -4405,7 +4374,7 @@
         <v>54.330000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -4420,7 +4389,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -4435,7 +4404,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -4443,7 +4412,7 @@
         <v>92.8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -4451,7 +4420,7 @@
         <v>148.93</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -4459,7 +4428,7 @@
         <v>100.42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -4467,7 +4436,7 @@
         <v>117.79</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -4488,7 +4457,7 @@
         <v>17.920000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -4503,7 +4472,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -4518,7 +4487,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -4526,7 +4495,7 @@
         <v>40.82</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -4534,7 +4503,7 @@
         <v>42.9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -4542,7 +4511,7 @@
         <v>33.26</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -4550,7 +4519,7 @@
         <v>53.76</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -4558,7 +4527,7 @@
         <v>78.290000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -4566,7 +4535,7 @@
         <v>71.459999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -4574,7 +4543,7 @@
         <v>47.63</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -4599,7 +4568,7 @@
         <v>385.60538461538454</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -4614,7 +4583,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -4629,7 +4598,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -4637,7 +4606,7 @@
         <v>419.97</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -4645,7 +4614,7 @@
         <v>404.56</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -4653,7 +4622,7 @@
         <v>569.35</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -4661,7 +4630,7 @@
         <v>413.33</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -4709,7 +4678,7 @@
         <v>256.19</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
@@ -4726,7 +4695,7 @@
         <v>137913.60000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
@@ -4741,7 +4710,7 @@
       </c>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -4756,7 +4725,7 @@
       </c>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
@@ -5262,11 +5231,11 @@
         <v>24833222.721799999</v>
       </c>
       <c r="E93" s="6">
-        <f>F93*5280</f>
-        <v>241296.00000000003</v>
-      </c>
-      <c r="F93" s="6">
-        <v>45.7</v>
+        <v>1191753.5115199999</v>
+      </c>
+      <c r="F93" s="1">
+        <f>E93/5280</f>
+        <v>225.71089233333333</v>
       </c>
       <c r="I93" s="1">
         <f>32259.562785/5280</f>
@@ -5289,8 +5258,7 @@
       <c r="D94" s="2">
         <v>56199751.679700002</v>
       </c>
-      <c r="E94" s="6"/>
-      <c r="F94" s="13"/>
+      <c r="E94" s="8"/>
     </row>
     <row r="95" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
@@ -5305,7 +5273,7 @@
       <c r="D95" s="2">
         <v>16877323.793400001</v>
       </c>
-      <c r="E95" s="6"/>
+      <c r="E95" s="8"/>
     </row>
     <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
@@ -5525,7 +5493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -5546,7 +5514,7 @@
         <v>78.97</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -5560,7 +5528,7 @@
         <v>9224.9699999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -5574,7 +5542,7 @@
         <v>8317.75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -5588,7 +5556,7 @@
         <v>12648.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -5602,7 +5570,7 @@
         <v>18130.2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -5610,7 +5578,7 @@
         <v>48.27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -5618,7 +5586,7 @@
         <v>37.85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -5626,7 +5594,7 @@
         <v>30.88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -5634,7 +5602,7 @@
         <v>27.69</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -5642,7 +5610,7 @@
         <v>24.53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -5650,7 +5618,7 @@
         <v>25.52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -5658,7 +5626,7 @@
         <v>45.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -5666,7 +5634,7 @@
         <v>26.63</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -5674,7 +5642,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -5682,7 +5650,7 @@
         <v>33.24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -5690,7 +5658,7 @@
         <v>20.93</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -5711,7 +5679,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -5725,7 +5693,7 @@
         <v>4827.1000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -5740,7 +5708,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -5748,7 +5716,7 @@
         <v>27.78</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -5756,7 +5724,7 @@
         <v>37.44</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -5764,7 +5732,7 @@
         <v>48.07</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -5772,7 +5740,7 @@
         <v>38.44</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -5780,7 +5748,7 @@
         <v>34.659999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -5788,7 +5756,7 @@
         <v>47.47</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -5796,7 +5764,7 @@
         <v>43.39</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -5804,7 +5772,7 @@
         <v>60.56</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -5821,7 +5789,7 @@
         <v>146836.79999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -5836,7 +5804,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -5851,7 +5819,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -5866,7 +5834,7 @@
       </c>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -5881,7 +5849,7 @@
       </c>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -5889,7 +5857,7 @@
         <v>44.49</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -5897,7 +5865,7 @@
         <v>49.23</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -5905,7 +5873,7 @@
         <v>40.67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -5913,7 +5881,7 @@
         <v>35.159999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -5921,7 +5889,7 @@
         <v>29.21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -5929,7 +5897,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -5937,7 +5905,7 @@
         <v>27.07</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -5945,7 +5913,7 @@
         <v>41.54</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -5953,7 +5921,7 @@
         <v>36.21</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -5961,7 +5929,7 @@
         <v>46.93</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
@@ -5969,7 +5937,7 @@
         <v>45.36</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -8715,7 +8683,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -8741,7 +8709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
@@ -8767,7 +8735,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>51</v>
       </c>
@@ -8793,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -8823,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>53</v>
       </c>

</xml_diff>